<commit_message>
new changes by list 12092021
</commit_message>
<xml_diff>
--- a/web/excel/kassa1.xlsx
+++ b/web/excel/kassa1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ишлар\МТД\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BA1455-36D1-4A08-B8E3-153AE79F1465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF99EFF-8951-4605-A29C-7AC1075FB798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$P$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$Q$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>№</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Қарз сумма</t>
+  </si>
+  <si>
+    <t>Тўланган сумма</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:V1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -544,14 +547,14 @@
     <col min="6" max="6" width="24.85546875" style="7" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" style="9" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="24.85546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" style="5" customWidth="1"/>
-    <col min="14" max="16" width="24.85546875" style="1" customWidth="1"/>
+    <col min="9" max="11" width="24.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="5" customWidth="1"/>
+    <col min="15" max="17" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="E1" s="7"/>
@@ -561,9 +564,10 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
-      <c r="M1" s="5"/>
+      <c r="L1" s="9"/>
+      <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:16" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
@@ -579,15 +583,16 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="2"/>
+      <c r="N2" s="6"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="E3" s="7"/>
@@ -597,9 +602,10 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
-      <c r="M3" s="5"/>
+      <c r="L3" s="9"/>
+      <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:16" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="27.6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -631,21 +637,24 @@
         <v>11</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kassir report excel file changed
</commit_message>
<xml_diff>
--- a/web/excel/kassa1.xlsx
+++ b/web/excel/kassa1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF99EFF-8951-4605-A29C-7AC1075FB798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247FA5B2-9891-4EB2-AC73-CBFDBC69477B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$Q$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$R$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>№</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Тўланган сумма</t>
+  </si>
+  <si>
+    <t>Тўлов тури</t>
   </si>
 </sst>
 </file>
@@ -93,12 +96,16 @@
       <sz val="14"/>
       <color rgb="FF003F2F"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF003F2F"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -531,10 +538,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -547,14 +554,14 @@
     <col min="6" max="6" width="24.85546875" style="7" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" style="9" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="24.85546875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="5" customWidth="1"/>
-    <col min="15" max="17" width="24.85546875" style="1" customWidth="1"/>
+    <col min="9" max="12" width="24.85546875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" style="5" customWidth="1"/>
+    <col min="16" max="18" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="E1" s="7"/>
@@ -565,9 +572,10 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
-      <c r="N1" s="5"/>
+      <c r="M1" s="9"/>
+      <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:17" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
@@ -584,15 +592,16 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="E3" s="7"/>
@@ -603,9 +612,10 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="N3" s="5"/>
+      <c r="M3" s="9"/>
+      <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:17" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="27.6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -637,24 +647,27 @@
         <v>11</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>